<commit_message>
Corrigido os seguintes itens: 1 - Problema em Estudo | 2 - Relevancia do trabalho | 3 - Objetivo do trabalho
</commit_message>
<xml_diff>
--- a/PLANILHA DE CORREÇOES DOCUMENTACAO.xlsx
+++ b/PLANILHA DE CORREÇOES DOCUMENTACAO.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32">
   <si>
     <t>Professor</t>
   </si>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>Mas quem é o cliente? Como seu trabalho é acadêmico a parte de requisitos não faz sentido.</t>
-  </si>
-  <si>
-    <t>Citar cliente em Problema Identificado ?</t>
   </si>
   <si>
     <t>Como requisitos foram levantados?</t>
@@ -123,10 +120,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;* #,##0_-;\-&quot;R$&quot;* #,##0_-;_-&quot;R$&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;R$&quot;* #,##0_-;\-&quot;R$&quot;* #,##0_-;_-&quot;R$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -137,6 +134,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -145,7 +157,61 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
@@ -154,7 +220,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -168,30 +234,38 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -199,83 +273,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -302,175 +299,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -487,6 +484,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -501,6 +507,36 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -523,32 +559,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -557,22 +569,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -592,148 +589,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1069,7 +1066,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D18:D19"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="4"/>
@@ -1195,7 +1192,7 @@
         <v>17</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1205,9 +1202,11 @@
       <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="1"/>
+      <c r="C8" s="1">
+        <v>25</v>
+      </c>
       <c r="D8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E8" s="1"/>
     </row>
@@ -1222,10 +1221,10 @@
         <v>45</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1239,7 +1238,7 @@
         <v>47</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E10" t="s">
         <v>8</v>
@@ -1256,7 +1255,7 @@
         <v>48</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E11" t="s">
         <v>8</v>
@@ -1273,7 +1272,7 @@
         <v>61</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E12" t="s">
         <v>8</v>
@@ -1290,7 +1289,7 @@
         <v>77</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E13" t="s">
         <v>8</v>
@@ -1307,7 +1306,7 @@
         <v>79</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E14" t="s">
         <v>8</v>
@@ -1324,7 +1323,7 @@
         <v>79</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E15" t="s">
         <v>8</v>
@@ -1341,7 +1340,7 @@
         <v>79</v>
       </c>
       <c r="D16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E16" t="s">
         <v>8</v>
@@ -1358,7 +1357,7 @@
         <v>95</v>
       </c>
       <c r="D17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E17" t="s">
         <v>8</v>
@@ -1375,7 +1374,7 @@
         <v>113</v>
       </c>
       <c r="D18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E18" t="s">
         <v>8</v>
@@ -1383,7 +1382,7 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
         <v>13</v>
@@ -1392,7 +1391,7 @@
         <v>105</v>
       </c>
       <c r="D19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E19" t="s">
         <v>8</v>
@@ -1400,7 +1399,7 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
         <v>13</v>
@@ -1409,7 +1408,7 @@
         <v>107</v>
       </c>
       <c r="D20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E20" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Finalizado Cap 3.4 | finalizado fluxograma | gerado versao final revisada | ajustado numercao de imagens
</commit_message>
<xml_diff>
--- a/PLANILHA DE CORREÇOES DOCUMENTACAO.xlsx
+++ b/PLANILHA DE CORREÇOES DOCUMENTACAO.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35">
   <si>
     <t>Professor</t>
   </si>
@@ -34,6 +34,9 @@
     <t>Status</t>
   </si>
   <si>
+    <t>Ação</t>
+  </si>
+  <si>
     <t>Mineda</t>
   </si>
   <si>
@@ -46,6 +49,9 @@
     <t>Concluído</t>
   </si>
   <si>
+    <t>-</t>
+  </si>
+  <si>
     <t>A palavra "guerras" já foi usado nessa frase. Reescreve e use pronome.</t>
   </si>
   <si>
@@ -73,13 +79,16 @@
     <t>Mas quem é o cliente? Como seu trabalho é acadêmico a parte de requisitos não faz sentido.</t>
   </si>
   <si>
+    <t>Alteração nos subCapitulos 1.1 e .12</t>
+  </si>
+  <si>
     <t>Como requisitos foram levantados?</t>
   </si>
   <si>
     <t>Onde está o código da roteirização?</t>
   </si>
   <si>
-    <t>Criar Subcapitulo para Implementaçao de Código de roteirização</t>
+    <t>Criacão do Subcapitulo 3.4</t>
   </si>
   <si>
     <t>No último usa ponto.</t>
@@ -120,10 +129,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;R$&quot;* #,##0_-;\-&quot;R$&quot;* #,##0_-;_-&quot;R$&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;* #,##0_-;\-&quot;R$&quot;* #,##0_-;_-&quot;R$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -131,6 +140,35 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -149,6 +187,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -165,6 +219,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -181,51 +250,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -243,22 +267,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -270,15 +286,8 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -293,49 +302,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -347,13 +446,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -365,115 +464,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -487,10 +502,60 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -526,45 +591,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -573,172 +599,164 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -1063,20 +1081,21 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="5"/>
   <cols>
     <col min="2" max="3" width="11.8571428571429" customWidth="1"/>
     <col min="4" max="4" width="78.1428571428571" customWidth="1"/>
-    <col min="5" max="5" width="28.4285714285714" customWidth="1"/>
+    <col min="5" max="5" width="11.2857142857143" customWidth="1"/>
+    <col min="6" max="6" width="30.1428571428571" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1092,326 +1111,386 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>16</v>
       </c>
       <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
       </c>
       <c r="C3">
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C5">
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1">
         <v>25</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>16</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C7" s="1">
         <v>25</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C8" s="1">
         <v>25</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="C9" s="1">
         <v>45</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C10">
         <v>47</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C11">
         <v>48</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C12">
         <v>61</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>23</v>
+      <c r="D12" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="E12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C13">
         <v>77</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>9</v>
+      </c>
+      <c r="F13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C14">
         <v>79</v>
       </c>
       <c r="D14" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C15">
         <v>79</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>9</v>
+      </c>
+      <c r="F15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C16">
         <v>79</v>
       </c>
       <c r="D16" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>9</v>
+      </c>
+      <c r="F16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C17">
         <v>95</v>
       </c>
       <c r="D17" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>9</v>
+      </c>
+      <c r="F17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C18">
         <v>113</v>
       </c>
       <c r="D18" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>9</v>
+      </c>
+      <c r="F18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C19">
         <v>105</v>
       </c>
       <c r="D19" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>9</v>
+      </c>
+      <c r="F19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C20">
         <v>107</v>
       </c>
       <c r="D20" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E20" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="F20" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>